<commit_message>
added DL on UML
</commit_message>
<xml_diff>
--- a/UserStories/UserStories.xlsx
+++ b/UserStories/UserStories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Documents\leaguePlatformWebApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\OneDrive\Documents\goalLine\goalLine_webApp\UserStories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E6B6B2-3209-46ED-9D6B-14DAD68EDEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FC6AFC-9255-4910-AC73-73DF68E4BD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-510" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
     <t>Epic</t>
   </si>
@@ -451,6 +451,18 @@
   </si>
   <si>
     <t>PUS-MPT-003</t>
+  </si>
+  <si>
+    <t>LEGEND</t>
+  </si>
+  <si>
+    <t>To Remove</t>
+  </si>
+  <si>
+    <t>Not Done Yet</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -488,7 +500,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,8 +555,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -759,49 +795,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -813,30 +831,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -849,6 +846,70 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,597 +1203,652 @@
     <col min="3" max="3" width="119.5703125" customWidth="1"/>
     <col min="4" max="4" width="57.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="16" t="s">
+      <c r="F2" s="43"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="36"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="10" t="s">
+      <c r="F3" s="43"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="17" t="s">
+      <c r="F4" s="43"/>
+      <c r="I4" s="44" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="44"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="36"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="17" t="s">
+      <c r="F5" s="43"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="36"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="9" t="s">
+      <c r="F6" s="43"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="36"/>
+      <c r="B7" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="16" t="s">
+      <c r="F7" s="43"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="36"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="5" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="16" t="s">
+      <c r="F8" s="43"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="36"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="16" t="s">
+      <c r="F9" s="43"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="36"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="16" t="s">
+      <c r="F10" s="43"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="36"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="10" t="s">
+      <c r="F11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="17" t="s">
+      <c r="F12" s="43"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="17" t="s">
+      <c r="F13" s="43"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="17" t="s">
+      <c r="F14" s="43"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="9" t="s">
+      <c r="F15" s="43"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="16" t="s">
+      <c r="F16" s="42"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="10" t="s">
+      <c r="F17" s="43"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="6" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="17" t="s">
+      <c r="F18" s="41"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="18" t="s">
+      <c r="F19" s="41"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="37"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="6" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="20" t="s">
+      <c r="F21" s="43"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="26"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="9" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="20" t="s">
+      <c r="F22" s="43"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="26"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="9" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="20" t="s">
+      <c r="F23" s="43"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="26"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="9" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="10" t="s">
+      <c r="F24" s="43"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="26"/>
+      <c r="B25" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E25" s="17" t="s">
+      <c r="E25" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="17" t="s">
+      <c r="F25" s="41"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="6" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="17" t="s">
+      <c r="F26" s="43"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="26"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="14" t="s">
+      <c r="F27" s="43"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="26"/>
+      <c r="B28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="9" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="10" t="s">
+      <c r="F28" s="41"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="26"/>
+      <c r="B29" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="17" t="s">
+      <c r="F29" s="41"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="17" t="s">
+      <c r="F30" s="41"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="26"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="18" t="s">
+      <c r="F31" s="41"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="17" t="s">
+      <c r="E32" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
+      <c r="F32" s="41"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="11" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="27" t="s">
+      <c r="F33" s="41"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="11" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27" t="s">
+      <c r="F34" s="41"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="32"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="39" t="s">
+      <c r="D35" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="11" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
-      <c r="B36" s="30" t="s">
+      <c r="F35" s="41"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="32"/>
+      <c r="B36" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="17" t="s">
+      <c r="F36" s="43"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="32"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E37" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="17" t="s">
+      <c r="F37" s="43"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="32"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="17" t="s">
+      <c r="F38" s="43"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="32"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
-      <c r="B40" s="26" t="s">
+      <c r="F39" s="43"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="32"/>
+      <c r="B40" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="39" t="s">
+      <c r="D40" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="11" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27" t="s">
+      <c r="F40" s="41"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="32"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="D41" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="E41" s="27" t="s">
+      <c r="E41" s="11" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="28"/>
-      <c r="C42" s="29" t="s">
+      <c r="F41" s="41"/>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="33"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="E42" s="29" t="s">
+      <c r="E42" s="12" t="s">
         <v>141</v>
       </c>
+      <c r="F42" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A21:A32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="B36:B39"/>
+  <mergeCells count="16">
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="B40:B42"/>
     <mergeCell ref="A33:A42"/>
     <mergeCell ref="B12:B15"/>
@@ -1743,6 +1859,11 @@
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A21:A32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B36:B39"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>